<commit_message>
C10001 input and output stored in different formats
</commit_message>
<xml_diff>
--- a/C10001_compare/C10001_annotated.xlsx
+++ b/C10001_compare/C10001_annotated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karen/workspaces/test_data_10_tables/C10001_compare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4837A870-2628-2147-A11F-00A9ACDA0674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86161C35-0604-0C4F-A0AE-7A1B34E14FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34960" yWindow="12560" windowWidth="23060" windowHeight="8680" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="C10001" sheetId="1" r:id="rId1"/>
@@ -587,12 +587,6 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -607,6 +601,12 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -933,539 +933,541 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <sheetData>
     <row r="1" spans="1:21" ht="18">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
     </row>
     <row r="2" spans="1:21" ht="18">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1">
-      <c r="B3" s="4"/>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1" t="s">
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1" t="s">
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1" t="s">
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1" t="s">
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1" t="s">
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
     </row>
     <row r="4" spans="1:21">
-      <c r="B4" s="4"/>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="5" t="s">
+      <c r="O4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="5" t="s">
+      <c r="P4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="Q4" s="5" t="s">
+      <c r="Q4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="R4" s="5" t="s">
+      <c r="R4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="S4" s="5" t="s">
+      <c r="S4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="T4" s="5" t="s">
+      <c r="T4" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="14">
-      <c r="B5" s="6">
+      <c r="B5" s="4">
         <v>2008</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="K5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="L5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="M5" s="7" t="s">
+      <c r="M5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="N5" s="7">
+      <c r="N5" s="5">
         <v>37</v>
       </c>
-      <c r="O5" s="7" t="s">
+      <c r="O5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="P5" s="7" t="s">
+      <c r="P5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="Q5" s="7" t="s">
+      <c r="Q5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="R5" s="7" t="s">
+      <c r="R5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="S5" s="7" t="s">
+      <c r="S5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="T5" s="7" t="s">
+      <c r="T5" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="14">
-      <c r="B6" s="6">
+      <c r="B6" s="4">
         <v>2007</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="K6" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="L6" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="M6" s="7" t="s">
+      <c r="M6" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="N6" s="7" t="s">
+      <c r="N6" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="O6" s="7" t="s">
+      <c r="O6" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="P6" s="7" t="s">
+      <c r="P6" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="Q6" s="7" t="s">
+      <c r="Q6" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="R6" s="7" t="s">
+      <c r="R6" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="S6" s="7" t="s">
+      <c r="S6" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="T6" s="7" t="s">
+      <c r="T6" s="5" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="14">
-      <c r="B7" s="6">
+      <c r="B7" s="4">
         <v>2006</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="K7" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="L7" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="M7" s="7" t="s">
+      <c r="M7" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="N7" s="7" t="s">
+      <c r="N7" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="O7" s="7" t="s">
+      <c r="O7" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="P7" s="7" t="s">
+      <c r="P7" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="Q7" s="7" t="s">
+      <c r="Q7" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="R7" s="7" t="s">
+      <c r="R7" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="S7" s="7" t="s">
+      <c r="S7" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="T7" s="7">
+      <c r="T7" s="5">
         <v>-548</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="14">
-      <c r="B8" s="6">
+      <c r="B8" s="4">
         <v>2005</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="J8" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="K8" s="7" t="s">
+      <c r="K8" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="L8" s="7" t="s">
+      <c r="L8" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="M8" s="7" t="s">
+      <c r="M8" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="N8" s="7" t="s">
+      <c r="N8" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="O8" s="7" t="s">
+      <c r="O8" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="P8" s="7" t="s">
+      <c r="P8" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="Q8" s="7" t="s">
+      <c r="Q8" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="R8" s="7" t="s">
+      <c r="R8" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="S8" s="7" t="s">
+      <c r="S8" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="T8" s="7">
+      <c r="T8" s="5">
         <v>-78</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="14">
-      <c r="B9" s="6">
+      <c r="B9" s="4">
         <v>2004</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="I9" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="J9" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="K9" s="7" t="s">
+      <c r="K9" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="L9" s="7" t="s">
+      <c r="L9" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="M9" s="7" t="s">
+      <c r="M9" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="N9" s="7" t="s">
+      <c r="N9" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="O9" s="7" t="s">
+      <c r="O9" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="P9" s="7" t="s">
+      <c r="P9" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="Q9" s="7" t="s">
+      <c r="Q9" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="R9" s="7" t="s">
+      <c r="R9" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="S9" s="7" t="s">
+      <c r="S9" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="T9" s="7">
+      <c r="T9" s="5">
         <v>-217</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="14">
-      <c r="B10" s="6">
+      <c r="B10" s="4">
         <v>2003</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="J10" s="7" t="s">
+      <c r="J10" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="K10" s="7" t="s">
+      <c r="K10" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="L10" s="7" t="s">
+      <c r="L10" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="M10" s="7" t="s">
+      <c r="M10" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="N10" s="7">
+      <c r="N10" s="5">
         <v>-939</v>
       </c>
-      <c r="O10" s="7" t="s">
+      <c r="O10" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="P10" s="7" t="s">
+      <c r="P10" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="Q10" s="7" t="s">
+      <c r="Q10" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="R10" s="7" t="s">
+      <c r="R10" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="S10" s="7" t="s">
+      <c r="S10" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="T10" s="7" t="s">
+      <c r="T10" s="5" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="14">
-      <c r="B11" s="6">
+      <c r="B11" s="4">
         <v>2002</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H11" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="I11" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="J11" s="7" t="s">
+      <c r="J11" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="K11" s="7" t="s">
+      <c r="K11" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="L11" s="7" t="s">
+      <c r="L11" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="M11" s="7" t="s">
+      <c r="M11" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="N11" s="7">
+      <c r="N11" s="5">
         <v>-882</v>
       </c>
-      <c r="O11" s="7" t="s">
+      <c r="O11" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="P11" s="7" t="s">
+      <c r="P11" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="Q11" s="7" t="s">
+      <c r="Q11" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="R11" s="7" t="s">
+      <c r="R11" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="S11" s="7" t="s">
+      <c r="S11" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="T11" s="7" t="s">
+      <c r="T11" s="5" t="s">
         <v>129</v>
       </c>
     </row>

</xml_diff>